<commit_message>
07.03.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/V48_&_L23i_imei.xlsx
+++ b/2020/V48_&_L23i_imei.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>v48</t>
   </si>
@@ -25,6 +25,18 @@
   </si>
   <si>
     <t>Date: 06.03.2020</t>
+  </si>
+  <si>
+    <t>Desh</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Natore</t>
+  </si>
+  <si>
+    <t>Jilani</t>
   </si>
 </sst>
 </file>
@@ -40,7 +52,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -59,8 +71,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -92,11 +140,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -108,6 +182,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -404,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C1:D32"/>
+  <dimension ref="C1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -418,217 +525,235 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4">
+    <row r="1" spans="3:5">
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="3:4">
+    <row r="2" spans="3:5">
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:4">
-      <c r="C3" s="2">
+    <row r="3" spans="3:5">
+      <c r="C3" s="5">
         <v>358932096676566</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>352573103347951</v>
       </c>
-    </row>
-    <row r="4" spans="3:4">
-      <c r="C4" s="2">
+      <c r="E3" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5">
+      <c r="C4" s="5">
         <v>358932096722600</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <v>352573103330528</v>
       </c>
-    </row>
-    <row r="5" spans="3:4">
-      <c r="C5" s="2">
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="3:5">
+      <c r="C5" s="5">
         <v>358932096722667</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="7">
         <v>352573103352969</v>
       </c>
-    </row>
-    <row r="6" spans="3:4">
-      <c r="C6" s="2">
+      <c r="E5" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5">
+      <c r="C6" s="5">
         <v>358932096736444</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="7">
         <v>352573103356614</v>
       </c>
-    </row>
-    <row r="7" spans="3:4">
-      <c r="C7" s="2">
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="3:5">
+      <c r="C7" s="5">
         <v>358932096756087</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="15">
         <v>352573103348512</v>
       </c>
-    </row>
-    <row r="8" spans="3:4">
-      <c r="C8" s="2">
+      <c r="E7" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5">
+      <c r="C8" s="5">
         <v>358932096756103</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="9">
         <v>352573103349163</v>
       </c>
-    </row>
-    <row r="9" spans="3:4">
-      <c r="C9" s="2">
+      <c r="E8" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5">
+      <c r="C9" s="5">
         <v>358932096760725</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="9">
         <v>352573103344529</v>
       </c>
-    </row>
-    <row r="10" spans="3:4">
-      <c r="C10" s="2">
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="3:5">
+      <c r="C10" s="5">
         <v>358932096760923</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="3:4">
-      <c r="C11" s="2">
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="3:5">
+      <c r="C11" s="5">
         <v>358932096765609</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="3:4">
-      <c r="C12" s="2">
+    <row r="12" spans="3:5">
+      <c r="C12" s="5">
         <v>358932096768165</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="3:4">
-      <c r="C13" s="2">
+    <row r="13" spans="3:5">
+      <c r="C13" s="3">
         <v>358932096768223</v>
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="3:4">
-      <c r="C14" s="2">
+    <row r="14" spans="3:5">
+      <c r="C14" s="3">
         <v>358932096772589</v>
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="3:4">
-      <c r="C15" s="2">
+    <row r="15" spans="3:5">
+      <c r="C15" s="3">
         <v>358932096786282</v>
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="3:4">
-      <c r="C16" s="2">
+    <row r="16" spans="3:5">
+      <c r="C16" s="3">
         <v>358932096787348</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="3:4">
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>358932096787389</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="3:4">
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>358932096787587</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="3:4">
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>358932096809225</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="3:4">
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>358932096830346</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="3:4">
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>358932096832029</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="3:4">
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>358932096901683</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="3:4">
-      <c r="C23" s="2">
+      <c r="C23" s="6">
         <v>358932096964228</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="3:4">
-      <c r="C24" s="2">
+      <c r="C24" s="6">
         <v>358932097105706</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="3:4">
-      <c r="C25" s="2">
+      <c r="C25" s="6">
         <v>358932096966769</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="3:4">
-      <c r="C26" s="2">
+      <c r="C26" s="6">
         <v>358932096935509</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="3:4">
-      <c r="C27" s="2">
+      <c r="C27" s="6">
         <v>358932097126405</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="3:4">
-      <c r="C28" s="2">
+      <c r="C28" s="6">
         <v>358932096963907</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="3:4">
-      <c r="C29" s="2">
+      <c r="C29" s="6">
         <v>358932096935483</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="3:4">
-      <c r="C30" s="2">
+      <c r="C30" s="6">
         <v>358932096935780</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="3:4">
-      <c r="C31" s="2">
+      <c r="C31" s="6">
         <v>358932096935947</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="3:4">
-      <c r="C32" s="2">
+      <c r="C32" s="6">
         <v>358932096964061</v>
       </c>
       <c r="D32" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>